<commit_message>
Add Project on the excel BOM
</commit_message>
<xml_diff>
--- a/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
+++ b/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Main_Board_Rev_A1!$A$1:$F$72</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="194">
   <si>
     <t>Qty</t>
   </si>
@@ -598,6 +598,12 @@
   </si>
   <si>
     <t>A1</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>WDY - Main Board</t>
   </si>
 </sst>
 </file>
@@ -1551,7 +1557,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F72"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,27 +1570,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>188</v>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="3">
         <f ca="1">TODAY()</f>
         <v>42709</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add power balance of the Main Board and update the BOM
</commit_message>
<xml_diff>
--- a/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
+++ b/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
@@ -1102,7 +1102,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1116,6 +1116,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1557,7 +1560,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,10 +1573,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update BOM of Main Board
</commit_message>
<xml_diff>
--- a/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
+++ b/WDY/Main_Board/Rev A1/Main_Board_Rev_A1_BOM.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_Board_Rev_A1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Main_Board_Rev_A1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Main_Board_Rev_A1!$A$1:$F$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Main_Board_Rev_A1!$A$1:$F$66</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="228">
   <si>
     <t>Qty</t>
   </si>
@@ -279,9 +280,6 @@
     <t>R8</t>
   </si>
   <si>
-    <t>4K87</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
@@ -372,12 +370,6 @@
     <t>Surface-mounting Switches Ideal for</t>
   </si>
   <si>
-    <t>BC-2-P</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>CMDSH2-3</t>
   </si>
   <si>
@@ -604,6 +596,117 @@
   </si>
   <si>
     <t>WDY - Main Board</t>
+  </si>
+  <si>
+    <t>Board Name</t>
+  </si>
+  <si>
+    <t>Main Board</t>
+  </si>
+  <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>OVS-0604</t>
+  </si>
+  <si>
+    <t>TC1264-3.3VDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLV313IDCKT  </t>
+  </si>
+  <si>
+    <t>TPL0401A-10DCKR</t>
+  </si>
+  <si>
+    <t>OVS-0608</t>
+  </si>
+  <si>
+    <t>MSTBA 2,5/ 2-G-5,08</t>
+  </si>
+  <si>
+    <t>MMBT2222ALT3G</t>
+  </si>
+  <si>
+    <t>G6K-2G-Y 24DC</t>
+  </si>
+  <si>
+    <t>ASE-12.000MHZ-LC-T</t>
+  </si>
+  <si>
+    <t>ASE-50.000MHZ-LC-T</t>
+  </si>
+  <si>
+    <t>MCMR06X1001FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X4701FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1002FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1201FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1501FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1801FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X2200FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X33R0FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X49R9FTL</t>
+  </si>
+  <si>
+    <t>MCMR06X000 PTL</t>
+  </si>
+  <si>
+    <t>MCMR06X1000FTL</t>
+  </si>
+  <si>
+    <t>Q13FC13500004 FC-135 32.768KHZ 12.5PF</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-B</t>
+  </si>
+  <si>
+    <t>MC0603B104K160CT</t>
+  </si>
+  <si>
+    <t>MC0603B183K160CT</t>
+  </si>
+  <si>
+    <t>MC0603B105K160CT</t>
+  </si>
+  <si>
+    <t>MC0603B225K6R3CT</t>
+  </si>
+  <si>
+    <t>MC0603X475K6R3CT</t>
+  </si>
+  <si>
+    <t>MC0603B472K500CT</t>
+  </si>
+  <si>
+    <t>MCMR06X60R4FTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F931A475MAA  </t>
+  </si>
+  <si>
+    <t>F931A106MAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3557  </t>
+  </si>
+  <si>
+    <t>UPS120E3/TR7</t>
   </si>
 </sst>
 </file>
@@ -746,7 +849,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -924,6 +1027,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1102,7 +1211,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1120,6 +1229,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1180,25 +1296,20 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1733550</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>41016</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="4320000" cy="877597"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{537F0C6E-59B5-4421-858F-142DAF2C16BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48620F5-BBCA-43EC-BEF6-1B36AB8EE948}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1221,8 +1332,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="3952875" cy="803016"/>
+          <a:off x="0" y="1"/>
+          <a:ext cx="4320000" cy="877597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1253,7 +1364,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1554,13 +1665,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A6:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="3">
+        <f ca="1">TODAY()</f>
+        <v>42711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,181 +1743,283 @@
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56" style="1" customWidth="1"/>
     <col min="6" max="6" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D2" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" s="3">
-        <f ca="1">TODAY()</f>
-        <v>42709</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="4">
+        <v>603</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <v>100</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="B10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="4">
-        <v>603</v>
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>19</v>
-      </c>
-      <c r="B12" s="4">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>14</v>
@@ -1753,18 +2028,21 @@
         <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>22</v>
@@ -1773,18 +2051,21 @@
         <v>23</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>6</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>22</v>
@@ -1793,76 +2074,90 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>22</v>
@@ -1871,296 +2166,341 @@
         <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
+      </c>
+      <c r="D22" s="4">
+        <v>2007041</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>2</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2007069</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>3</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="4">
+        <v>2007100</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="4">
+        <v>2007130</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1647397</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>2</v>
+      </c>
+      <c r="B27" s="4">
+        <v>220</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="4" t="s">
+      <c r="E27" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>2</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
-        <v>2</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>5</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="4">
-        <v>2007041</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>2</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>61</v>
+        <v>1</v>
+      </c>
+      <c r="B28" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3000</v>
       </c>
       <c r="D28" s="4">
-        <v>2007069</v>
+        <v>3000</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>3</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>63</v>
+      <c r="B29" s="4">
+        <v>33</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D29" s="4">
-        <v>2007100</v>
+        <v>22</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="4">
-        <v>2007130</v>
+        <v>14</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1647397</v>
+        <v>34</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>2</v>
-      </c>
-      <c r="B32" s="4">
-        <v>220</v>
+        <v>1</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="G32" s="2">
+        <v>7447713047</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>1</v>
       </c>
-      <c r="B33" s="4">
-        <v>3000</v>
-      </c>
-      <c r="C33" s="4">
-        <v>3000</v>
-      </c>
-      <c r="D33" s="4">
-        <v>3000</v>
+      <c r="B33" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>3</v>
-      </c>
-      <c r="B34" s="4">
-        <v>33</v>
+        <v>4</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>22</v>
@@ -2169,98 +2509,113 @@
         <v>23</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>15</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
         <v>2</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>1</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>1</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
-        <v>1</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>4</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>81</v>
+      <c r="B39" s="4">
+        <v>60.4</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>22</v>
@@ -2269,657 +2624,622 @@
         <v>23</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>22</v>
+        <v>97</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
+        <v>1</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
         <v>2</v>
       </c>
-      <c r="B44" s="4">
-        <v>60</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <v>1</v>
-      </c>
       <c r="B45" s="4" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
+        <v>1</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>1</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>1</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>4</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
         <v>2</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
-        <v>1</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>1</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>1</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="B52" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>1</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>1</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>1</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="E55" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>1</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>1</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>1</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
         <v>2</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
-        <v>1</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
-        <v>1</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
-        <v>1</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
-        <v>1</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
-        <v>1</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4">
-        <v>1</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
-        <v>4</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="B59" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
         <v>2</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
-        <v>1</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
-        <v>1</v>
-      </c>
       <c r="B60" s="4" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>1</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>1</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>1</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="F65" s="4"/>
+      <c r="G65" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
-        <v>3</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
-        <v>1</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
-        <v>1</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
-        <v>1</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
-        <v>1</v>
-      </c>
-      <c r="B71" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="F71" s="4"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="4">
-        <v>1</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="F72" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>